<commit_message>
included python answers, requirements file, changes to MySQL answers and new sql database script for mysql
</commit_message>
<xml_diff>
--- a/PythonTestQuestions/Privia Family Medicine 113018.xlsx
+++ b/PythonTestQuestions/Privia Family Medicine 113018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewclark/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/libloaner-mac16/Documents/GitHub/data_engineering_assessment/PythonTestQuestions/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{319681C2-B83E-7842-8BFC-425B96B2D42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2340" windowWidth="28800" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$4:$M$4</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1127,7 +1128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1209,6 +1210,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1476,7 +1480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>